<commit_message>
Needs ALU, Memory, Control Signal Generator
created CS generator, cleaned coded, modularized, major component
declaration, reformatted.

NOT functioning, need to finish CS generator
</commit_message>
<xml_diff>
--- a/OPCodesRev02.xlsx
+++ b/OPCodesRev02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>Format</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>R[3]&lt;- R[1]+R[2]</t>
+  </si>
+  <si>
+    <t>R[4]&lt;- R[4]+R[4]</t>
   </si>
   <si>
     <t>Format B</t>
@@ -453,7 +456,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -478,11 +481,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -492,10 +495,6 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="6" fontId="0" numFmtId="164" xfId="0">
@@ -896,10 +895,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B12" activeCellId="0" pane="topLeft" sqref="B12"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B24" activeCellId="0" pane="topLeft" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -977,15 +976,15 @@
         <v>69</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6" t="e">
+        <v>4</v>
+      </c>
+      <c r="E5" s="0" t="e">
         <f aca="false">BIN2DEC(E7)</f>
         <v>#VALUE!</v>
       </c>
@@ -996,17 +995,17 @@
       </c>
       <c r="B6" s="0" t="str">
         <f aca="false">DEC2HEX(B5)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">DEC2HEX(C5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">DEC2HEX(D5)</f>
-        <v>3</v>
-      </c>
-      <c r="E6" s="6" t="e">
+        <v>4</v>
+      </c>
+      <c r="E6" s="0" t="e">
         <f aca="false">BIN2HEX(E7)</f>
         <v>#VALUE!</v>
       </c>
@@ -1017,23 +1016,23 @@
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">DEC2BIN(B5,B4)</f>
-        <v>00001</v>
+        <v>00100</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">DEC2BIN(C5,C4)</f>
-        <v>00010</v>
+        <v>00100</v>
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">DEC2BIN(D5,D4)</f>
-        <v>00011</v>
-      </c>
-      <c r="E7" s="7" t="str">
+        <v>00100</v>
+      </c>
+      <c r="E7" s="6" t="str">
         <f aca="false">SUBSTITUTE(C9,"_","")</f>
         <v>00000000001000000</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="8">
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
@@ -1045,10 +1044,10 @@
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="10">
-      <c r="E10" s="7"/>
+      <c r="E10" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
@@ -1056,15 +1055,15 @@
       </c>
       <c r="B11" s="4" t="str">
         <f aca="false">B7&amp;C7&amp;D7&amp;E7</f>
-        <v>00001000100001100000000001000000</v>
+        <v>00100001000010000000000001000000</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="6" t="e">
-        <f aca="false">BIN2HEX(B11)</f>
+      <c r="B12" s="0" t="e">
+        <f aca="false">BIN2DEC(B11)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1090,6 +1089,14 @@
       </c>
       <c r="B25" s="0" t="n">
         <v>142999616</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="26">
+      <c r="A26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>554172480</v>
       </c>
     </row>
   </sheetData>
@@ -1110,7 +1117,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B24" activeCellId="0" pane="topLeft" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1129,10 +1136,10 @@
         <v>56</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>58</v>
@@ -1147,7 +1154,7 @@
         <v>61</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>62</v>
@@ -1161,13 +1168,13 @@
         <v>64</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="4">
@@ -1200,7 +1207,7 @@
       <c r="D5" s="5" t="n">
         <v>9191</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="0" t="n">
         <f aca="false">BIN2DEC(E7)</f>
         <v>34</v>
       </c>
@@ -1221,7 +1228,7 @@
         <f aca="false">DEC2HEX(D5)</f>
         <v>23E7</v>
       </c>
-      <c r="E6" s="6" t="str">
+      <c r="E6" s="0" t="str">
         <f aca="false">BIN2HEX(E7)</f>
         <v>22</v>
       </c>
@@ -1247,22 +1254,22 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="8">
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="10" t="n">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>100010</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="10">
-      <c r="E10" s="7"/>
+      <c r="E10" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
@@ -1277,7 +1284,7 @@
       <c r="A12" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="11" t="e">
+      <c r="B12" s="10" t="e">
         <f aca="false">BIN2DEC(B11)</f>
         <v>#VALUE!</v>
       </c>
@@ -1292,7 +1299,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>38336994</v>

</xml_diff>